<commit_message>
add draft sex extension for version 6.1.0
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -2543,12 +2543,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Birth Sex Extension</t>
+          <t>US Core Patient Profile | US Core Sex Extension</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Birth Sex</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>US Core Birth Sex Extension</t>
+          <t>US Core Sex Extension</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -2573,12 +2573,12 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Birth Sex Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Date of Birth</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>US Core Birth Sex Extension</t>
+          <t>Patient.birthDate</t>
         </is>
       </c>
       <c r="G74" t="inlineStr"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Date of Birth</t>
+          <t>Date of Death</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Patient.birthDate</t>
+          <t>Patient.deceased[x]</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>
@@ -2633,22 +2633,22 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Date of Death</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>US Core Race Extension</t>
         </is>
       </c>
       <c r="G76" t="inlineStr"/>
@@ -2663,12 +2663,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Ethnicity Extension</t>
         </is>
       </c>
       <c r="G77" t="inlineStr"/>
@@ -2693,12 +2693,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Tribal Affiliation</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>US Core Ethnicity Extension</t>
+          <t>US Core Tibal Affiliation Extension</t>
         </is>
       </c>
       <c r="G78" t="inlineStr"/>
@@ -2723,12 +2723,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Tribal Affiliation</t>
+          <t>Gender Identity</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>US Core Tibal Affiliation Extension</t>
+          <t>Gender Identity Extension</t>
         </is>
       </c>
       <c r="G79" t="inlineStr"/>
@@ -2753,22 +2753,22 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Sexual Orientation</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Gender Identity Extension</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G80" t="inlineStr"/>
@@ -2783,22 +2783,22 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Preferred Language</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.communication</t>
         </is>
       </c>
       <c r="G81" t="inlineStr"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Preferred Language</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="G82" t="inlineStr"/>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Previous Address</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Previous Address</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2933,22 +2933,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Phone Number</t>
+          <t>Related Person's Name</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>RelatedPerson.name</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Related Person's Name</t>
+          <t>Related Person's Relationship</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>RelatedPerson.name</t>
+          <t>RelatedPerson.relationship</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -2993,22 +2993,22 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Related Person's Relationship</t>
+          <t>Occupation</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>RelatedPerson.relationship</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G88" t="inlineStr"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>Occupation Industry</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3045,39 +3045,35 @@
       <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr"/>
+      <c r="A90" t="n">
+        <v>14</v>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Occupation Industry</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>14</v>
-      </c>
+      <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr">
         <is>
           <t>Problems</t>
@@ -3088,7 +3084,11 @@
           <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Date of Resolution</t>
+        </is>
+      </c>
       <c r="E91" t="inlineStr">
         <is>
           <t>US Core Condition Problems and Health Concerns Profile</t>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Condition.abatement[x]</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Date of Resolution</t>
+          <t>Date of Diagnosis</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Condition.abatement[x]</t>
+          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Date of Diagnosis</t>
+          <t>SDOH Problems/Health Concerns</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3156,54 +3156,46 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr"/>
+      <c r="A94" t="n">
+        <v>15</v>
+      </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>SDOH Problems/Health Concerns</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
+          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Procedure, ServiceRequest</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>15</v>
-      </c>
+      <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr">
         <is>
           <t>Procedures</t>
@@ -3211,14 +3203,22 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Procedure</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Procedure, ServiceRequest</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="G95" t="inlineStr"/>
@@ -3233,22 +3233,22 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Procedure</t>
+          <t>Reason for Referral</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Procedure</t>
+          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -3263,69 +3263,73 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Reason for Referral</t>
+          <t>SDOH Interventions</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
+          <t>ServiceRequest, Procedure</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr"/>
+      <c r="A98" t="n">
+        <v>16</v>
+      </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>SDOH Interventions</t>
-        </is>
-      </c>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>ServiceRequest, Procedure</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>See Screening and Assessments Guidance</t>
+          <t>See Basic Provenance Guidance</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>screening-and-assessments.html</t>
+          <t>basic-provenance.html</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>16</v>
-      </c>
+      <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr">
         <is>
           <t>Provenance</t>
@@ -3336,7 +3340,11 @@
           <t>US Core Provenance Profile</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Author Time Stamp</t>
+        </is>
+      </c>
       <c r="E99" t="inlineStr">
         <is>
           <t>US Core Provenance Profile</t>
@@ -3344,19 +3352,11 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>See Basic Provenance Guidance</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>basic-provenance.html</t>
-        </is>
-      </c>
+          <t>Provenance.recorded</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Author Time Stamp</t>
+          <t>Author Organization</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3382,46 +3382,42 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Provenance.recorded</t>
+          <t>Provenance.agent</t>
         </is>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr"/>
+      <c r="A101" t="n">
+        <v>17</v>
+      </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Author Organization</t>
-        </is>
-      </c>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Provenance.agent</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
     </row>
     <row r="102">
-      <c r="A102" t="n">
-        <v>17</v>
-      </c>
+      <c r="A102" t="inlineStr"/>
       <c r="B102" t="inlineStr">
         <is>
           <t>Unique Device Identifier(s)</t>
@@ -3432,7 +3428,11 @@
           <t>US Core Implantable Device Profile</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+        </is>
+      </c>
       <c r="E102" t="inlineStr">
         <is>
           <t>US Core Implantable Device Profile</t>
@@ -3447,39 +3447,31 @@
       <c r="H102" t="inlineStr"/>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr"/>
+      <c r="A103" t="n">
+        <v>18</v>
+      </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Vital Signs</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
+          <t>US Core Vital Signs Profile</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
     </row>
     <row r="104">
-      <c r="A104" t="n">
-        <v>18</v>
-      </c>
+      <c r="A104" t="inlineStr"/>
       <c r="B104" t="inlineStr">
         <is>
           <t>Vital Signs</t>
@@ -3487,11 +3479,19 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>US Core Vital Signs Profile</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Diastolic blood pressure</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+        </is>
+      </c>
       <c r="F104" t="inlineStr">
         <is>
           <t>Observation</t>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Diastolic blood pressure</t>
+          <t>Systolic blood pressure</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3539,17 +3539,17 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Systolic blood pressure</t>
+          <t>Body height</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3569,17 +3569,17 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Body height</t>
+          <t>Body weight</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Body weight</t>
+          <t>Heart rate</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3629,17 +3629,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Heart rate</t>
+          <t>Respiratory rate</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3659,17 +3659,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Respiratory rate</t>
+          <t>Body temperature</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3689,17 +3689,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Body temperature</t>
+          <t>Pulse oximetry</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Pulse oximetry</t>
+          <t>Inhaled oxygen concentration</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3749,17 +3749,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Inhaled oxygen concentration</t>
+          <t>BMI Percentile (2-20 years old)</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>BMI Percentile (2-20 years old)</t>
+          <t>Weight-for-length Percentile (Birth - 36 months)</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3809,17 +3809,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3829,36 +3829,6 @@
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Vital Signs</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
apply USCDI v4 Location changes part 1
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -552,13 +552,13 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Reaction</t>
+          <t>Substance (Non-Medication)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>AllergyIntolerance.reaction</t>
+          <t>AllergyIntolerance.code</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -568,23 +568,23 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Assessment and Plan of Treatment</t>
+          <t>Allergies and Intolerances</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile | US Core Simple Observation Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>US Core CarePlan Profile</t>
-        </is>
-      </c>
+          <t>US Core AllergyIntolerance Profile</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Reaction</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">CarePlan, Observation, </t>
+          <t>AllergyIntolerance.reaction</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -599,18 +599,18 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>US Core CarePlan Profile | US Core Simple Observation Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>US Core CarePlan Profile</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Assessment and Plan of Treatment</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CarePlan</t>
+          <t xml:space="preserve">CarePlan, Observation, </t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -625,84 +625,80 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core CarePlan Profile</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SDOH Assessment</t>
+          <t>Assessment and Plan of Treatment</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
+          <t>CarePlan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Assessment and Plan of Treatment</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>SDOH Assessment</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="10">
+      <c r="A10" t="n">
         <v>2</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Care Team Members</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>US Core CareTeam Profile</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
         <is>
           <t>US Core CareTeam Profile</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>CareTeam.participant</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Care Team Members</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>US Core CareTeam Profile</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Practitioner.name, RelatedPerson.name</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -722,17 +718,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>US Core Practitioner Profile| US Core Patient Profile</t>
+          <t>US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Practitioner.identifier</t>
+          <t>Practitioner.name, RelatedPerson.name</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -752,17 +748,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
+          <t>US Core Practitioner Profile| US Core Patient Profile</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>PractitionerRole.address, Practitioner.address, RelatedPerson.address</t>
+          <t>Practitioner.identifier</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -782,7 +778,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Telecom</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -792,7 +788,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>PractitionerRole.telecom, Practitioner.telecom, RelatedPerson.telecom</t>
+          <t>PractitionerRole.address, Practitioner.address, RelatedPerson.address</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -812,48 +808,56 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Role</t>
+          <t>Telecom</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
+          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>CareTeam.participant.role</t>
+          <t>PractitionerRole.telecom, Practitioner.telecom, RelatedPerson.telecom</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>3</v>
-      </c>
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Clinical Notes</t>
+          <t>Care Team Members</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+          <t>US Core CareTeam Profile</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>US Core CareTeam Profile</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
+          <t>CareTeam.participant.role</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Clinical Notes</t>
@@ -861,22 +865,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Consultation Note</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>US Core DocumentReference Profile</t>
-        </is>
-      </c>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>DocumentReference</t>
+          <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -896,7 +892,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Discharge Summary Note</t>
+          <t>Consultation Note</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -926,7 +922,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>History &amp; Physical</t>
+          <t>Discharge Summary Note</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -951,22 +947,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Imaging Narrative</t>
+          <t>History &amp; Physical</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
+          <t>DocumentReference</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -986,7 +982,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Laboratory Report Narrative</t>
+          <t>Imaging Narrative</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1016,7 +1012,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Pathology Report Narrative</t>
+          <t>Laboratory Report Narrative</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1046,7 +1042,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Procedure Note</t>
+          <t>Pathology Report Narrative</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1071,78 +1067,82 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Procedure Note</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>DocumentReference,DiagnosticReport</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Clinical Notes</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Progress Note</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>See Clinical Notes Guidance</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>clinical-notes.html</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="25">
+      <c r="A25" t="n">
         <v>4</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>Clinical Tests</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Clinical Tests</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Observation, DiagnosticReport</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Clinical Tests</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Clinical Test</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Clinical Test Result/Report</t>
+          <t>Clinical Test</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1181,12 +1181,10 @@
       <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>5</v>
-      </c>
+      <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging</t>
+          <t>Clinical Tests</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1194,7 +1192,11 @@
           <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Clinical Test Result/Report</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
@@ -1205,7 +1207,9 @@
       <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>5</v>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>Diagnostic Imaging</t>
@@ -1216,16 +1220,8 @@
           <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Diagnostic Imaging Test</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
-        </is>
-      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
@@ -1248,7 +1244,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging Result/Report</t>
+          <t>Diagnostic Imaging Test</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1265,35 +1261,39 @@
       <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>6</v>
-      </c>
+      <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Diagnostic Imaging</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
+          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Diagnostic Imaging Result/Report</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Observation, DiagnosticReport</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="n">
+        <v>6</v>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>Encounter</t>
@@ -1304,11 +1304,7 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
           <t>US Core Encounter Profile</t>
@@ -1316,7 +1312,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Encounter.type</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -1331,22 +1327,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Condition.code</t>
+          <t>Encounter.type</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1361,22 +1357,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Diagnosis</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Encounter.period</t>
+          <t>Condition.code</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1396,7 +1392,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1406,7 +1402,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Encounter.location.location</t>
+          <t>Encounter.period</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1426,7 +1422,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1436,123 +1432,141 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Encounter.hospitalization.dischargeDisposition</t>
+          <t>Encounter.location.location</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>7</v>
-      </c>
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Disposition</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Goal</t>
+          <t>Encounter.hospitalization.dischargeDisposition</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="n">
+        <v>7</v>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Patient Goals</t>
-        </is>
-      </c>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Goal</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+          <t>Location.identifier</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>See Facility Information Guidance</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>StructureDefinition-us-core-location.html</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>SDOH Goals</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Goal</t>
+          <t>Location.identifier</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>See Screening and Assessments Guidance</t>
+          <t>See Facility Information Guidance</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>screening-and-assessments.html</t>
+          <t>StructureDefinition-us-core-location.html</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>8</v>
-      </c>
+      <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Health Insurance Information</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Coverage</t>
+          <t>Location.type</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1562,57 +1576,51 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Health Insurance Information</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Coverage Status</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Coverage.status + Coverage.period</t>
+          <t>Location.name</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="n">
+        <v>8</v>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Health Insurance Information</t>
+          <t>Goals</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Coverage Type</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Coverage.type</t>
+          <t>Goal</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1622,27 +1630,27 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Health Insurance Information</t>
+          <t>Goals</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Relationship to Subscriber</t>
+          <t>Patient Goals</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Coverage,relationship</t>
+          <t>Goal</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1652,57 +1660,59 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Goals</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>SDOH Goals</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Goal</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>9</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>Health Insurance Information</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Member Identifier</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Coverage.identifier</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Health Insurance Information</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Subscriber Identifier</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Coverage.subscriberId</t>
+          <t>Coverage</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1722,7 +1732,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Group Number</t>
+          <t>Coverage Status</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1732,7 +1742,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Coverage.class</t>
+          <t>Coverage.status + Coverage.period</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1752,7 +1762,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Payer Identifier</t>
+          <t>Coverage Type</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1762,35 +1772,37 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Coverage.payer</t>
+          <t>Coverage.type</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>9</v>
-      </c>
+      <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>Relationship to Subscriber</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>US Core Coverage Profile</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Observation,Condition,QuestionnaireResponse</t>
+          <t>Coverage,relationship</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1800,27 +1812,27 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Health Concerns</t>
+          <t>Member Identifier</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Coverage.identifier</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1830,65 +1842,57 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Functional Status</t>
+          <t>Subscriber Identifier</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Coverage.subscriberId</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Disability Status</t>
+          <t>Group Number</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Coverage.class</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -1898,34 +1902,36 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Mental/Cognitive Status</t>
+          <t>Payer Identifier</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Coverage.payer</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" t="n">
+        <v>10</v>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>Health Status/Assessments</t>
@@ -1933,22 +1939,18 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Pregnancy Status</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
-        </is>
-      </c>
+          <t>Health Status/Assessments</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -1963,96 +1965,120 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Smoking Status</t>
+          <t>Health Concerns</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>10</v>
-      </c>
+      <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Immunizations</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Functional Status</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
+          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Immunization</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Immunizations</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Disability Status</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Immunization</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>11</v>
-      </c>
+      <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Mental/Cognitive Status</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport,Specimen</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -2062,27 +2088,27 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Tests</t>
+          <t>Pregnancy Status</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Observation.code, DiagnosticReport.code</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -2092,57 +2118,55 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Smoking Status Observation Profile</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Values/Results</t>
+          <t>Smoking Status</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Smoking Status Observation Profile</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Observation.value[x], DiagnosticReport.result</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
+      <c r="A59" t="n">
+        <v>11</v>
+      </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Immunizations</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Specimen Type</t>
-        </is>
-      </c>
+          <t>US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
+          <t>US Core Immunization Profile</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Observation.specimen, Specimen</t>
+          <t>Immunization</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -2152,27 +2176,19 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Immunizations</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Result Status</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
+          <t>US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Observation.status, DiagnosticReport.status</t>
+          <t>Immunization</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -2184,19 +2200,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>MedicationRequest, MedicationDispense, Medication</t>
+          <t>Observation, DiagnosticReport,Specimen</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -2206,65 +2222,57 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>US Core Medication Profile | US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Tests</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Medication.code, MedicationRequest.medication[x]</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>See Medication List Guidance</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>medication-list.html</t>
-        </is>
-      </c>
+          <t>Observation.code, DiagnosticReport.code</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Dose</t>
+          <t>Values/Results</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+          <t>Observation.value[x], DiagnosticReport.result</t>
         </is>
       </c>
       <c r="G63" t="inlineStr"/>
@@ -2274,27 +2282,27 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Dose Unit of Measure</t>
+          <t>Specimen Type</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+          <t>Observation.specimen, Specimen</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -2304,34 +2312,36 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Indication</t>
+          <t>Result Status</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>MedicationRequest.reasonCode, Medication, MedicationreasonReference</t>
+          <t>Observation.status, DiagnosticReport.status</t>
         </is>
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr"/>
+      <c r="A66" t="n">
+        <v>13</v>
+      </c>
       <c r="B66" t="inlineStr">
         <is>
           <t>Medications</t>
@@ -2339,76 +2349,82 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>US Core Medication Dispense Profile</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Fill Status</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>US Core Medication Profile|  US Core Medication Dispense Profile</t>
-        </is>
-      </c>
+          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>MedicationDispense</t>
+          <t>MedicationRequest, MedicationDispense, Medication</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>13</v>
-      </c>
+      <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+          <t>US Core Medication Profile | US Core Medication Request Profile</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Medications</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>US Core Medication Profile|  US Core Medication Request Profile</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Patient, Observation</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
+          <t>Medication.code, MedicationRequest.medication[x]</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>See Medication List Guidance</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>medication-list.html</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Dose</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
         </is>
       </c>
       <c r="G68" t="inlineStr"/>
@@ -2418,27 +2434,27 @@
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Dose Unit of Measure</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Patient.name.family</t>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
         </is>
       </c>
       <c r="G69" t="inlineStr"/>
@@ -2448,27 +2464,27 @@
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>Indication</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Request Profile</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Patient.name</t>
+          <t>MedicationRequest.reasonCode, Medication, MedicationreasonReference</t>
         </is>
       </c>
       <c r="G70" t="inlineStr"/>
@@ -2478,34 +2494,36 @@
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Dispense Profile</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Middle Name (including middle initial)</t>
+          <t>Fill Status</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Profile|  US Core Medication Dispense Profile</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>MedicationDispense</t>
         </is>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
+      <c r="A72" t="n">
+        <v>14</v>
+      </c>
       <c r="B72" t="inlineStr">
         <is>
           <t>Patient Demographics</t>
@@ -2513,22 +2531,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Suffix</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
+          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Patient.name.suffix</t>
+          <t>Patient, Observation</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
@@ -2543,12 +2553,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Sex Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2558,7 +2568,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>US Core Sex Extension</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -2578,7 +2588,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Date of Birth</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2588,7 +2598,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Patient.birthDate</t>
+          <t>Patient.name.family</t>
         </is>
       </c>
       <c r="G74" t="inlineStr"/>
@@ -2608,7 +2618,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Date of Death</t>
+          <t>Previous Name</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2618,7 +2628,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>Patient.name</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>
@@ -2633,12 +2643,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Middle Name (including middle initial)</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2648,7 +2658,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="G76" t="inlineStr"/>
@@ -2663,12 +2673,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Suffix</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2678,7 +2688,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>US Core Ethnicity Extension</t>
+          <t>Patient.name.suffix</t>
         </is>
       </c>
       <c r="G77" t="inlineStr"/>
@@ -2693,12 +2703,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+          <t>US Core Patient Profile | US Core Sex Extension</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Tribal Affiliation</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2708,7 +2718,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>US Core Tibal Affiliation Extension</t>
+          <t>US Core Sex Extension</t>
         </is>
       </c>
       <c r="G78" t="inlineStr"/>
@@ -2723,12 +2733,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Date of Birth</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2738,7 +2748,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Gender Identity Extension</t>
+          <t>Patient.birthDate</t>
         </is>
       </c>
       <c r="G79" t="inlineStr"/>
@@ -2753,22 +2763,22 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Date of Death</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.deceased[x]</t>
         </is>
       </c>
       <c r="G80" t="inlineStr"/>
@@ -2783,22 +2793,22 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Preferred Language</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
+          <t>US Core Race Extension</t>
         </is>
       </c>
       <c r="G81" t="inlineStr"/>
@@ -2813,22 +2823,22 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>US Core Ethnicity Extension</t>
         </is>
       </c>
       <c r="G82" t="inlineStr"/>
@@ -2843,22 +2853,22 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Tribal Affiliation</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Previous Address</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>US Core Tibal Affiliation Extension</t>
         </is>
       </c>
       <c r="G83" t="inlineStr"/>
@@ -2873,22 +2883,22 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Gender Identity</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>Gender Identity Extension</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -2903,22 +2913,22 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Phone Number</t>
+          <t>Sexual Orientation</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G85" t="inlineStr"/>
@@ -2933,22 +2943,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Related Person's Name</t>
+          <t>Preferred Language</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>RelatedPerson.name</t>
+          <t>Patient.communication</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -2963,22 +2973,22 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Related Person's Relationship</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>RelatedPerson.relationship</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -2993,22 +3003,22 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>Previous Address</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="G88" t="inlineStr"/>
@@ -3023,50 +3033,52 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Occupation Industry</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>14</v>
-      </c>
+      <c r="A90" t="inlineStr"/>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="G90" t="inlineStr"/>
@@ -3076,27 +3088,27 @@
       <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Date of Resolution</t>
+          <t>Related Person's Name</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Condition.abatement[x]</t>
+          <t>RelatedPerson.name</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -3106,27 +3118,27 @@
       <c r="A92" t="inlineStr"/>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Date of Diagnosis</t>
+          <t>Related Person's Relationship</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
+          <t>RelatedPerson.relationship</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -3136,89 +3148,85 @@
       <c r="A93" t="inlineStr"/>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>SDOH Problems/Health Concerns</t>
+          <t>Occupation</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>15</v>
-      </c>
+      <c r="A94" t="inlineStr"/>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Occupation Industry</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Procedure, ServiceRequest</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr"/>
+      <c r="A95" t="n">
+        <v>15</v>
+      </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Procedure</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Procedure</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="G95" t="inlineStr"/>
@@ -3228,27 +3236,27 @@
       <c r="A96" t="inlineStr"/>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Reason for Referral</t>
+          <t>Date of Resolution</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
+          <t>Condition.abatement[x]</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -3258,101 +3266,89 @@
       <c r="A97" t="inlineStr"/>
       <c r="B97" t="inlineStr">
         <is>
+          <t>Problems</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Date of Diagnosis</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Problems</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>SDOH Problems/Health Concerns</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>16</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
           <t>Procedures</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>SDOH Interventions</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>ServiceRequest, Procedure</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>16</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>See Basic Provenance Guidance</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>basic-provenance.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Provenance</t>
-        </is>
-      </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Author Time Stamp</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
+          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Provenance.recorded</t>
+          <t>Procedure, ServiceRequest</t>
         </is>
       </c>
       <c r="G99" t="inlineStr"/>
@@ -3362,55 +3358,57 @@
       <c r="A100" t="inlineStr"/>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Author Organization</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Provenance.agent</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="n">
-        <v>17</v>
-      </c>
+      <c r="A101" t="inlineStr"/>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr"/>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Reason for Referral</t>
+        </is>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -3420,81 +3418,101 @@
       <c r="A102" t="inlineStr"/>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+          <t>SDOH Interventions</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Device</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
+          <t>ServiceRequest, Procedure</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>US Core Vital Signs Profile</t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr"/>
-      <c r="H103" t="inlineStr"/>
+          <t>Provenance</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>See Basic Provenance Guidance</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>basic-provenance.html</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr"/>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Diastolic blood pressure</t>
+          <t>Author Time Stamp</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Provenance.recorded</t>
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
@@ -3504,57 +3522,55 @@
       <c r="A105" t="inlineStr"/>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Systolic blood pressure</t>
+          <t>Author Organization</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Provenance.agent</t>
         </is>
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
+      <c r="A106" t="n">
+        <v>18</v>
+      </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Body height</t>
-        </is>
-      </c>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="G106" t="inlineStr"/>
@@ -3564,34 +3580,36 @@
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Body weight</t>
+          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr"/>
+      <c r="A108" t="n">
+        <v>19</v>
+      </c>
       <c r="B108" t="inlineStr">
         <is>
           <t>Vital Signs</t>
@@ -3599,19 +3617,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Heart rate</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
-        </is>
-      </c>
+          <t>US Core Vital Signs Profile</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr">
         <is>
           <t>Observation</t>
@@ -3629,17 +3639,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Respiratory rate</t>
+          <t>Diastolic blood pressure</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3659,17 +3669,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Body temperature</t>
+          <t>Systolic blood pressure</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3689,17 +3699,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Pulse oximetry</t>
+          <t>Body height</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3719,17 +3729,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Inhaled oxygen concentration</t>
+          <t>Body weight</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -3749,17 +3759,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>BMI Percentile (2-20 years old)</t>
+          <t>Heart rate</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3779,17 +3789,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+          <t>Respiratory rate</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3809,17 +3819,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+          <t>Body temperature</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3829,6 +3839,156 @@
       </c>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Pulse oximetry</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Inhaled oxygen concentration</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>BMI Percentile (2-20 years old)</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
update USCDI Location part 2
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -2371,7 +2371,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>US Core Medication Profile | US Core Medication Request Profile</t>
+          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core Medication Request Profile</t>
+          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>US Core Medication Request Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>US Core Medication Dispense Profile</t>
+          <t>US Core MedicationDispense Profile</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core Medication Dispense Profile</t>
+          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">

</xml_diff>

<commit_message>
update the uscsdi table and the uscore maps
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -1332,7 +1332,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Encounter.type</t>
+          <t>Encounter.identifier</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1357,22 +1357,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Condition.code</t>
+          <t>Encounter.type</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1387,22 +1387,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Diagnosis</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Encounter.period</t>
+          <t>Condition.code</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Encounter.location.location</t>
+          <t>Encounter.period</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1462,65 +1462,57 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Encounter.hospitalization.dischargeDisposition</t>
+          <t>Encounter.location.location</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Encounter</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Disposition</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Encounter.hospitalization.dischargeDisposition</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
         <v>7</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>Facility Information</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>US Core Location Profile</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Location.identifier</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>See Facility Information Guidance</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>StructureDefinition-us-core-location.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Facility Information</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>US Core Location Profile</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Identifier</t>
-        </is>
-      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
           <t>US Core Location Profile</t>
@@ -1556,7 +1548,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1566,11 +1558,19 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Location.type</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+          <t>Location.identifier</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>See Facility Information Guidance</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>StructureDefinition-us-core-location.html</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1596,38 +1596,46 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Location.name</t>
+          <t>Location.type</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>8</v>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Goal</t>
+          <t>Location.name</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="n">
+        <v>8</v>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>Goals</t>
@@ -1638,16 +1646,8 @@
           <t>US Core Goal Profile</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Patient Goals</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
           <t>Goal</t>
@@ -1670,79 +1670,79 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
+          <t>Patient Goals</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Goal</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Goals</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>SDOH Goals</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>US Core Goal Profile</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>Goal</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row r="45">
+      <c r="A45" t="n">
         <v>9</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>Health Insurance Information</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
         <is>
           <t>Coverage</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Health Insurance Information</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Coverage Status</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Coverage.status + Coverage.period</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Coverage Type</t>
+          <t>Coverage Status</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Coverage.type</t>
+          <t>Coverage.status + Coverage.period</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Relationship to Subscriber</t>
+          <t>Coverage Type</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Coverage,relationship</t>
+          <t>Coverage.type</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Member Identifier</t>
+          <t>Relationship to Subscriber</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Coverage.identifier</t>
+          <t>Coverage,relationship</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Subscriber Identifier</t>
+          <t>Member Identifier</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Coverage.subscriberId</t>
+          <t>Coverage.identifier</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Group Number</t>
+          <t>Subscriber Identifier</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Coverage.class</t>
+          <t>Coverage.subscriberId</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Payer Identifier</t>
+          <t>Group Number</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1922,42 +1922,46 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Coverage.payer</t>
+          <t>Coverage.class</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>10</v>
-      </c>
+      <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Coverage Profile</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>Payer Identifier</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>US Core Coverage Profile</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Observation,Condition,QuestionnaireResponse</t>
+          <t>Coverage.payer</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
+      <c r="A53" t="n">
+        <v>10</v>
+      </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>Health Status/Assessments</t>
@@ -1965,22 +1969,18 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Health Concerns</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
+          <t>Health Status/Assessments</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -1995,34 +1995,26 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Functional Status</t>
+          <t>Health Concerns</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -2038,7 +2030,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Disability Status</t>
+          <t>Functional Status</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2051,8 +2043,16 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Mental/Cognitive Status</t>
+          <t>Disability Status</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2093,17 +2093,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Pregnancy Status</t>
+          <t>Mental/Cognitive Status</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2123,17 +2123,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Smoking Status</t>
+          <t>Pregnancy Status</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2145,35 +2145,39 @@
       <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>11</v>
-      </c>
+      <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Immunizations</t>
+          <t>Health Status/Assessments</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
+          <t>US Core Smoking Status Observation Profile</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Smoking Status</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
+          <t>US Core Smoking Status Observation Profile</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Immunization</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
+      <c r="A60" t="n">
+        <v>11</v>
+      </c>
       <c r="B60" t="inlineStr">
         <is>
           <t>Immunizations</t>
@@ -2185,7 +2189,11 @@
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>US Core Immunization Profile</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>Immunization</t>
@@ -2195,31 +2203,31 @@
       <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>12</v>
-      </c>
+      <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Immunizations</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
+          <t>US Core Immunization Profile</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport,Specimen</t>
+          <t>Immunization</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr"/>
+      <c r="A62" t="n">
+        <v>12</v>
+      </c>
       <c r="B62" t="inlineStr">
         <is>
           <t>Laboratory</t>
@@ -2227,22 +2235,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Tests</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Observation.code, DiagnosticReport.code</t>
+          <t>Observation, DiagnosticReport,Specimen</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Values/Results</t>
+          <t>Tests</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Observation.value[x], DiagnosticReport.result</t>
+          <t>Observation.code, DiagnosticReport.code</t>
         </is>
       </c>
       <c r="G63" t="inlineStr"/>
@@ -2287,22 +2287,22 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Specimen Type</t>
+          <t>Values/Results</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Observation.specimen, Specimen</t>
+          <t>Observation.value[x], DiagnosticReport.result</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -2317,53 +2317,61 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Result Status</t>
+          <t>Specimen Type</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Observation.status, DiagnosticReport.status</t>
+          <t>Observation.specimen, Specimen</t>
         </is>
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>13</v>
-      </c>
+      <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Result Status</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>MedicationRequest, MedicationDispense, Medication</t>
+          <t>Observation.status, DiagnosticReport.status</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr"/>
+      <c r="A67" t="n">
+        <v>13</v>
+      </c>
       <c r="B67" t="inlineStr">
         <is>
           <t>Medications</t>
@@ -2371,34 +2379,18 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Medications</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
-        </is>
-      </c>
+          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Medication.code, MedicationRequest.medication[x]</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>See Medication List Guidance</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>medication-list.html</t>
-        </is>
-      </c>
+          <t>MedicationRequest, MedicationDispense, Medication</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
@@ -2409,26 +2401,34 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Dose</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
+          <t>Medication.code, MedicationRequest.medication[x]</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>See Medication List Guidance</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>medication-list.html</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Dose Unit of Measure</t>
+          <t>Dose</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Indication</t>
+          <t>Dose Unit of Measure</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>MedicationRequest.reasonCode, Medication, MedicationreasonReference</t>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
         </is>
       </c>
       <c r="G70" t="inlineStr"/>
@@ -2499,53 +2499,61 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>US Core MedicationDispense Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Fill Status</t>
+          <t>Indication</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>MedicationDispense</t>
+          <t>MedicationRequest.reasonCode, Medication, MedicationreasonReference</t>
         </is>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>14</v>
-      </c>
+      <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+          <t>US Core MedicationDispense Profile</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Fill Status</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Patient, Observation</t>
+          <t>MedicationDispense</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="n">
+        <v>14</v>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>Patient Demographics</t>
@@ -2553,22 +2561,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
+          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>Patient, Observation</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Patient.name.family</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="G74" t="inlineStr"/>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Patient.name</t>
+          <t>Patient.name.family</t>
         </is>
       </c>
       <c r="G75" t="inlineStr"/>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Middle Name (including middle initial)</t>
+          <t>Previous Name</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>Patient.name</t>
         </is>
       </c>
       <c r="G76" t="inlineStr"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Suffix</t>
+          <t>Middle Name (including middle initial)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Patient.name.suffix</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="G77" t="inlineStr"/>
@@ -2703,12 +2703,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Sex Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Suffix</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>US Core Sex Extension</t>
+          <t>Patient.name.suffix</t>
         </is>
       </c>
       <c r="G78" t="inlineStr"/>
@@ -2733,22 +2733,22 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Sex Extension</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Date of Birth</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Patient.birthDate</t>
+          <t>US Core Sex Extension</t>
         </is>
       </c>
       <c r="G79" t="inlineStr"/>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Date of Death</t>
+          <t>Date of Birth</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>Patient.birthDate</t>
         </is>
       </c>
       <c r="G80" t="inlineStr"/>
@@ -2793,12 +2793,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Date of Death</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>Patient.deceased[x]</t>
         </is>
       </c>
       <c r="G81" t="inlineStr"/>
@@ -2823,12 +2823,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+          <t>US Core Race Extension</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Race</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>US Core Ethnicity Extension</t>
+          <t>US Core Race Extension</t>
         </is>
       </c>
       <c r="G82" t="inlineStr"/>
@@ -2853,12 +2853,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Tribal Affiliation</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>US Core Tibal Affiliation Extension</t>
+          <t>US Core Ethnicity Extension</t>
         </is>
       </c>
       <c r="G83" t="inlineStr"/>
@@ -2883,12 +2883,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Tribal Affiliation</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Gender Identity Extension</t>
+          <t>US Core Tibal Affiliation Extension</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -2913,22 +2913,22 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Gender Identity</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Gender Identity Extension</t>
         </is>
       </c>
       <c r="G85" t="inlineStr"/>
@@ -2943,22 +2943,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Preferred Language</t>
+          <t>Sexual Orientation</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Preferred Language</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>Patient.communication</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Previous Address</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Previous Address</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="G89" t="inlineStr"/>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Phone Number</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3093,22 +3093,22 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Related Person's Name</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>RelatedPerson.name</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Related Person's Relationship</t>
+          <t>Related Person's Name</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>RelatedPerson.relationship</t>
+          <t>RelatedPerson.name</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -3153,22 +3153,22 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>Related Person's Relationship</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>RelatedPerson.relationship</t>
         </is>
       </c>
       <c r="G93" t="inlineStr"/>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Occupation Industry</t>
+          <t>Occupation</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3205,35 +3205,39 @@
       <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>15</v>
-      </c>
+      <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr"/>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Occupation Industry</t>
+        </is>
+      </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr"/>
+      <c r="A96" t="n">
+        <v>15</v>
+      </c>
       <c r="B96" t="inlineStr">
         <is>
           <t>Problems</t>
@@ -3244,11 +3248,7 @@
           <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Date of Resolution</t>
-        </is>
-      </c>
+      <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
           <t>US Core Condition Problems and Health Concerns Profile</t>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Condition.abatement[x]</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Date of Diagnosis</t>
+          <t>Date of Resolution</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3286,7 +3286,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
+          <t>Condition.abatement[x]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr"/>
@@ -3306,79 +3306,79 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
+          <t>Date of Diagnosis</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Problems</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
           <t>SDOH Problems/Health Concerns</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E99" t="inlineStr">
         <is>
           <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
+      <c r="F99" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G99" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H98" t="inlineStr">
+      <c r="H99" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="n">
+    <row r="100">
+      <c r="A100" t="n">
         <v>16</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B100" t="inlineStr">
         <is>
           <t>Procedures</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr">
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
         <is>
           <t>Procedure, ServiceRequest</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr"/>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Procedures</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Procedure</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>Procedure</t>
         </is>
       </c>
       <c r="G100" t="inlineStr"/>
@@ -3393,22 +3393,22 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Reason for Referral</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -3423,154 +3423,156 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>SDOH Interventions</t>
+          <t>Time of Procedure</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>ServiceRequest, Procedure</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Procedure.pertormed[x],DiagnosticReport.effective[x],Immunization.occurrence[x]</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
     </row>
     <row r="103">
-      <c r="A103" t="n">
-        <v>17</v>
-      </c>
+      <c r="A103" t="inlineStr"/>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr"/>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Reason for Referral</t>
+        </is>
+      </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>See Basic Provenance Guidance</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>basic-provenance.html</t>
-        </is>
-      </c>
+          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr"/>
       <c r="B104" t="inlineStr">
         <is>
+          <t>Procedures</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>SDOH Interventions</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>ServiceRequest, Procedure</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>17</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
           <t>Provenance</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>US Core Provenance Profile</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr">
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Provenance</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>See Basic Provenance Guidance</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>basic-provenance.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Provenance</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
         <is>
           <t>Author Time Stamp</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
+      <c r="E106" t="inlineStr">
         <is>
           <t>US Core Provenance Profile</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
+      <c r="F106" t="inlineStr">
         <is>
           <t>Provenance.recorded</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Author Organization</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Provenance.agent</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>18</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier(s)</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Device</t>
         </is>
       </c>
       <c r="G106" t="inlineStr"/>
@@ -3580,27 +3582,27 @@
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+          <t>Author Organization</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>Provenance.agent</t>
         </is>
       </c>
       <c r="G107" t="inlineStr"/>
@@ -3608,23 +3610,27 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>US Core Vital Signs Profile</t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="G108" t="inlineStr"/>
@@ -3634,34 +3640,36 @@
       <c r="A109" t="inlineStr"/>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Diastolic blood pressure</t>
+          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr"/>
+      <c r="A110" t="n">
+        <v>19</v>
+      </c>
       <c r="B110" t="inlineStr">
         <is>
           <t>Vital Signs</t>
@@ -3669,19 +3677,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Systolic blood pressure</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
-        </is>
-      </c>
+          <t>US Core Vital Signs Profile</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr">
         <is>
           <t>Observation</t>
@@ -3699,17 +3699,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Body height</t>
+          <t>Diastolic blood pressure</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3729,17 +3729,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Body weight</t>
+          <t>Systolic blood pressure</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -3759,17 +3759,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Heart rate</t>
+          <t>Body height</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3789,17 +3789,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Respiratory rate</t>
+          <t>Body weight</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3819,17 +3819,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Body temperature</t>
+          <t>Heart rate</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3849,17 +3849,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Pulse oximetry</t>
+          <t>Respiratory rate</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3879,17 +3879,17 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Inhaled oxygen concentration</t>
+          <t>Body temperature</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3909,17 +3909,17 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>BMI Percentile (2-20 years old)</t>
+          <t>Pulse oximetry</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3939,17 +3939,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+          <t>Inhaled oxygen concentration</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -3969,17 +3969,17 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+          <t>BMI Percentile (2-20 years old)</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -3989,6 +3989,66 @@
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Add USCDI Medication Data Class and Laboratory Data Class
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -448,15 +448,20 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>extension</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>fhir_path</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>comment_link</t>
         </is>
@@ -478,13 +483,14 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>AllergyIntolerance</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -504,13 +510,14 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>AllergyIntolerance.code</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -530,13 +537,14 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>AllergyIntolerance.code</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -556,13 +564,14 @@
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>AllergyIntolerance.code</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -582,13 +591,14 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>AllergyIntolerance.reaction</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -608,13 +618,14 @@
           <t>US Core CarePlan Profile</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t xml:space="preserve">CarePlan, Observation, </t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -634,13 +645,14 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>CarePlan</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -660,17 +672,18 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
@@ -696,13 +709,14 @@
           <t>US Core CareTeam Profile</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
         <is>
           <t>CareTeam.participant</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -726,13 +740,14 @@
           <t>US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Practitioner.name, RelatedPerson.name</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -756,13 +771,14 @@
           <t>US Core Practitioner Profile| US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Practitioner.identifier</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -786,13 +802,14 @@
           <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>PractitionerRole.address, Practitioner.address, RelatedPerson.address</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -816,13 +833,14 @@
           <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
         <is>
           <t>PractitionerRole.telecom, Practitioner.telecom, RelatedPerson.telecom</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -846,13 +864,14 @@
           <t>US Core CareTeam Profile</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
         <is>
           <t>CareTeam.participant.role</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -870,13 +889,14 @@
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -900,13 +920,14 @@
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -930,13 +951,14 @@
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
         <is>
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -960,13 +982,14 @@
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
         <is>
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -990,13 +1013,14 @@
           <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
         <is>
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1020,13 +1044,14 @@
           <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
         <is>
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1050,13 +1075,14 @@
           <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
         <is>
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -1080,13 +1106,14 @@
           <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
         <is>
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -1110,17 +1137,18 @@
           <t>US Core DocumentReference Profile</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
         <is>
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>See Clinical Notes Guidance</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>clinical-notes.html</t>
         </is>
@@ -1146,13 +1174,14 @@
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -1172,13 +1201,14 @@
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -1198,13 +1228,14 @@
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1222,13 +1253,14 @@
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -1252,13 +1284,14 @@
           <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -1282,13 +1315,14 @@
           <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1310,13 +1344,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
         <is>
           <t>Encounter</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -1340,13 +1375,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
         <is>
           <t>Encounter.identifier</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -1370,13 +1406,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
         <is>
           <t>Encounter.type</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -1400,13 +1437,14 @@
           <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
         <is>
           <t>Condition.code</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -1430,13 +1468,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
         <is>
           <t>Encounter.period</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -1460,13 +1499,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
         <is>
           <t>Encounter.location.location</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -1490,13 +1530,14 @@
           <t>US Core Encounter Profile</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
         <is>
           <t>Encounter.hospitalization.dischargeDisposition</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1518,17 +1559,18 @@
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
         <is>
           <t>Location.identifier</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>See Facility Information Guidance</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>StructureDefinition-us-core-location.html</t>
         </is>
@@ -1556,17 +1598,18 @@
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
         <is>
           <t>Location.identifier</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>See Facility Information Guidance</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>StructureDefinition-us-core-location.html</t>
         </is>
@@ -1594,13 +1637,14 @@
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
         <is>
           <t>Location.type</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -1624,13 +1668,14 @@
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
         <is>
           <t>Location.name</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1648,13 +1693,14 @@
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
         <is>
           <t>Goal</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -1678,13 +1724,14 @@
           <t>US Core Goal Profile</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
         <is>
           <t>Goal</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -1708,17 +1755,18 @@
           <t>US Core Goal Profile</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
         <is>
           <t>Goal</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
@@ -1740,13 +1788,14 @@
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
         <is>
           <t>Coverage</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -1770,13 +1819,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
         <is>
           <t>Coverage.status + Coverage.period</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -1800,13 +1850,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
         <is>
           <t>Coverage.type</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -1830,13 +1881,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
         <is>
           <t>Coverage,relationship</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -1860,13 +1912,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
         <is>
           <t>Coverage.identifier</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -1890,13 +1943,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
         <is>
           <t>Coverage.subscriberId</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -1920,13 +1974,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
         <is>
           <t>Coverage.class</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr"/>
@@ -1950,13 +2005,14 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
         <is>
           <t>Coverage.payer</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1978,13 +2034,14 @@
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr">
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
         <is>
           <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>
@@ -2008,13 +2065,14 @@
           <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -2038,17 +2096,18 @@
           <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>See Screening and Assessments Guidance</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="I55" t="inlineStr">
         <is>
           <t>screening-and-assessments.html</t>
         </is>
@@ -2076,13 +2135,14 @@
           <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -2106,13 +2166,14 @@
           <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr"/>
@@ -2136,13 +2197,14 @@
           <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
@@ -2166,13 +2228,14 @@
           <t>US Core Smoking Status Observation Profile</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2194,13 +2257,14 @@
           <t>US Core Immunization Profile</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
         <is>
           <t>Immunization</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr"/>
@@ -2216,13 +2280,14 @@
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr">
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
         <is>
           <t>Immunization</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2240,13 +2305,14 @@
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr">
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
         <is>
           <t>Observation, DiagnosticReport,Specimen</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -2270,13 +2336,14 @@
           <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
         <is>
           <t>Observation.code, DiagnosticReport.code</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr"/>
@@ -2300,13 +2367,14 @@
           <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
         <is>
           <t>Observation.value[x], DiagnosticReport.result</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr"/>
@@ -2330,13 +2398,14 @@
           <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
         <is>
           <t>Observation.specimen, Specimen</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr"/>
@@ -2360,459 +2429,479 @@
           <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
         <is>
           <t>Observation.status, DiagnosticReport.status</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>13</v>
-      </c>
+      <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>MedicationRequest, MedicationDispense, Medication</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
+          <t>US Core Laboratory Result Observation Profile</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Result Unit of Measure</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>US Core Laboratory Result Observation Profile</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>(Observation.value.ofType(Quantity)).code</t>
+        </is>
+      </c>
       <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Result Reference Range</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Medication.code, MedicationRequest.medication[x]</t>
-        </is>
-      </c>
+          <t>US Core Laboratory Result Observation Profile</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>See Medication List Guidance</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>medication-list.html</t>
-        </is>
-      </c>
+          <t>Observation.referenceRange</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Dose</t>
+          <t>Result Interpretation</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr"/>
+          <t>US Core Laboratory Result Observation Profile</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Observation.interpretation</t>
+        </is>
+      </c>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Dose Unit of Measure</t>
+          <t>Specimen Identifier</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr"/>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Specimen.identifier</t>
+        </is>
+      </c>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Indication</t>
+          <t>Specimen Source Site</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>MedicationRequest.reasonCode, Medication, MedicationreasonReference</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr"/>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Specimen.collection.bodySite</t>
+        </is>
+      </c>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>US Core MedicationDispense Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Fill Status</t>
+          <t>Specimen Condition Acceptability</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>MedicationDispense</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr"/>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Specimen.condition</t>
+        </is>
+      </c>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
+          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Patient, Observation</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>MedicationRequest, MedicationDispense, Medication</t>
+        </is>
+      </c>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Patient.name.given</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
+          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Medication.code, MedicationRequest.medication[x]</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>See Medication List Guidance</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>medication-list.html</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Dose</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Patient.name.family</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+        </is>
+      </c>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>Dose Unit of Measure</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Patient.name</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+        </is>
+      </c>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr"/>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Middle Name (including middle initial)</t>
+          <t>Indication</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Patient.name.given</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>MedicationRequest.reasonCode | Medication.reasonReference</t>
+        </is>
+      </c>
       <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Suffix</t>
+          <t>Medication Instructions</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Patient.name.suffix</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>MedicationRequest.dosageInstruction</t>
+        </is>
+      </c>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Sex Extension</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Medication Adherence</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>US Core Sex Extension</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr"/>
+          <t>US Core Medication Adherence Extension</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>MedicationRequest.extension.where(url='Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-medication-adherence')</t>
+        </is>
+      </c>
       <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
+          <t>Medications</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>US Core MedicationDispense Profile</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Fill Status</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>MedicationDispense</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>14</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
           <t>Patient Demographics</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Date of Birth</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Patient.birthDate</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr"/>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Patient Demographics</t>
-        </is>
-      </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Date of Death</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Patient.deceased[x]</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr"/>
+          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Patient, Observation</t>
+        </is>
+      </c>
       <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr"/>
@@ -2823,12 +2912,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2836,13 +2925,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>US Core Race Extension</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Patient.name.given</t>
+        </is>
+      </c>
       <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
@@ -2853,12 +2943,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2866,13 +2956,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>US Core Ethnicity Extension</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Patient.name.family</t>
+        </is>
+      </c>
       <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr"/>
@@ -2883,12 +2974,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Tribal Affiliation</t>
+          <t>Previous Name</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2896,13 +2987,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>US Core Tibal Affiliation Extension</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr"/>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Patient.name</t>
+        </is>
+      </c>
       <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr"/>
@@ -2913,12 +3005,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Middle Name (including middle initial)</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2926,13 +3018,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Gender Identity Extension</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Patient.name.given</t>
+        </is>
+      </c>
       <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr"/>
@@ -2943,26 +3036,27 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Suffix</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Patient.name.suffix</t>
+        </is>
+      </c>
       <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -2973,26 +3067,31 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Sex Extension</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Preferred Language</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr"/>
+          <t>US Core Sex Extension</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-sex')</t>
+        </is>
+      </c>
       <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr"/>
@@ -3008,7 +3107,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Date of Birth</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3016,13 +3115,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Patient.address</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Patient.birthDate</t>
+        </is>
+      </c>
       <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -3038,7 +3138,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Previous Address</t>
+          <t>Date of Death</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3046,13 +3146,14 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Patient.address</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Patient.deceased[x]</t>
+        </is>
+      </c>
       <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr"/>
@@ -3063,26 +3164,31 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr"/>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-race')</t>
+        </is>
+      </c>
       <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -3093,26 +3199,31 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Phone Number</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr"/>
+          <t>US Core Ethnicity Extension</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity')</t>
+        </is>
+      </c>
       <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr"/>
@@ -3123,26 +3234,31 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Related Person's Name</t>
+          <t>Tribal Affiliation</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>RelatedPerson.name</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr"/>
+          <t>US Core Tibal Affiliation Extension</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-tribal-affiliation')</t>
+        </is>
+      </c>
       <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -3153,26 +3269,31 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Related Person's Relationship</t>
+          <t>Gender Identity</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>RelatedPerson.relationship</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr"/>
+          <t>Gender Identity Extension</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-genderIdentity')</t>
+        </is>
+      </c>
       <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr"/>
@@ -3183,26 +3304,27 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>Sexual Orientation</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
+          <t>US Core Observation Sexual Orientation Profile</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -3213,722 +3335,750 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Occupation Industry</t>
+          <t>Preferred Language</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Patient.communication</t>
+        </is>
+      </c>
       <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="n">
-        <v>15</v>
-      </c>
+      <c r="A96" t="inlineStr"/>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Patient.address</t>
+        </is>
+      </c>
       <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Date of Resolution</t>
+          <t>Previous Address</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>Condition.abatement[x]</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Patient.address</t>
+        </is>
+      </c>
       <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Date of Diagnosis</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Choice of assertedDate Extension, Condition.onset[x], or Condition.onsetDate</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Patient.telecom</t>
+        </is>
+      </c>
       <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>SDOH Problems/Health Concerns</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Condition</t>
-        </is>
-      </c>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr">
         <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Patient.telecom</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" t="n">
-        <v>16</v>
-      </c>
+      <c r="A100" t="inlineStr"/>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>Procedure, ServiceRequest</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr"/>
+          <t>US Core RelatedPerson Profile</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Related Person's Name</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>US Core RelatedPerson Profile</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>RelatedPerson.name</t>
+        </is>
+      </c>
       <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr"/>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Procedure</t>
+          <t>Related Person's Relationship</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Procedure</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr"/>
+          <t>US Core RelatedPerson Profile</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>RelatedPerson.relationship</t>
+        </is>
+      </c>
       <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr"/>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Time of Procedure</t>
+          <t>Occupation</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Procedure.pertormed[x],DiagnosticReport.effective[x],Immunization.occurrence[x]</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr"/>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
       <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Reason for Referral</t>
+          <t>Occupation Industry</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr"/>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
       <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr"/>
+      <c r="A104" t="n">
+        <v>15</v>
+      </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>SDOH Interventions</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>ServiceRequest, Procedure</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr">
         <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
     </row>
     <row r="105">
-      <c r="A105" t="n">
-        <v>17</v>
-      </c>
+      <c r="A105" t="inlineStr"/>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr"/>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Date of Resolution</t>
+        </is>
+      </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Provenance</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr">
         <is>
-          <t>See Basic Provenance Guidance</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>basic-provenance.html</t>
-        </is>
-      </c>
+          <t>Condition.abatement[x]</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr"/>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Author Time Stamp</t>
+          <t>Date of Diagnosis</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Provenance.recorded</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr"/>
+          <t>assertedDate Extension</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Condition.extension.where(url='http://hl7.org/fhir/StructureDefinition/condition-assertedDate') |  Condition.onset[x] | Condition.onsetDate</t>
+        </is>
+      </c>
       <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Author Organization</t>
+          <t>SDOH Problems/Health Concerns</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Provenance.agent</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Device</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Procedure, ServiceRequest</t>
+        </is>
+      </c>
       <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr"/>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Device</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr"/>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Procedure</t>
+        </is>
+      </c>
       <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" t="n">
-        <v>19</v>
-      </c>
+      <c r="A110" t="inlineStr"/>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>US Core Vital Signs Profile</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr"/>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr"/>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Time of Procedure</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Procedure.pertormed[x],DiagnosticReport.effective[x],Immunization.occurrence[x]</t>
+        </is>
+      </c>
       <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr"/>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Diastolic blood pressure</t>
+          <t>Reason for Referral</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr"/>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
+        </is>
+      </c>
       <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr"/>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Systolic blood pressure</t>
+          <t>SDOH Interventions</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
+          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>ServiceRequest, Procedure</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr"/>
+      <c r="A113" t="n">
+        <v>17</v>
+      </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Body height</t>
-        </is>
-      </c>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Provenance</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>See Basic Provenance Guidance</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>basic-provenance.html</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Body weight</t>
+          <t>Author Time Stamp</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr"/>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Provenance.recorded</t>
+        </is>
+      </c>
       <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr"/>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Heart rate</t>
+          <t>Author Organization</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr"/>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Provenance.agent</t>
+        </is>
+      </c>
       <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr"/>
+      <c r="A116" t="n">
+        <v>18</v>
+      </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Unique Device Identifier(s)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Respiratory rate</t>
-        </is>
-      </c>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr"/>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Device</t>
+        </is>
+      </c>
       <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr"/>
       <c r="B117" t="inlineStr">
         <is>
+          <t>Unique Device Identifier(s)</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Device</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>19</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
           <t>Vital Signs</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Body temperature</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>US Core Vital Signs Profile</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Vital Signs</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Pulse oximetry</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr"/>
@@ -3939,26 +4089,27 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Inhaled oxygen concentration</t>
+          <t>Average Blood Pressure</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
+          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr"/>
@@ -3969,26 +4120,27 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>BMI Percentile (2-20 years old)</t>
+          <t>Diastolic blood pressure</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr"/>
@@ -3999,26 +4151,27 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+          <t>Systolic blood pressure</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr"/>
@@ -4029,26 +4182,306 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
+          <t xml:space="preserve">US Core Body Height Profile </t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Body height</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Body Height Profile </t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Heart rate</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Respiratory rate</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Body temperature</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Pulse oximetry</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Inhaled oxygen concentration</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>BMI Percentile (2-20 years old)</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
           <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr">
+      <c r="D131" t="inlineStr">
         <is>
           <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr">
+      <c r="E131" t="inlineStr">
         <is>
           <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
+      <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
add goal QA and USCDI table updates
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -601,27 +601,29 @@
       <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Assessment and Plan of Treatment</t>
+          <t>Care Team Members</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile | US Core Simple Observation Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core CareTeam Profile</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile</t>
+          <t>US Core CareTeam Profile</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">CarePlan, Observation, </t>
+          <t>CareTeam.participant</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -631,24 +633,28 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Assessment and Plan of Treatment</t>
+          <t>Care Team Members</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile</t>
+          <t>US Core CareTeam Profile</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Assessment and Plan of Treatment</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CarePlan</t>
+          <t>Practitioner.name, RelatedPerson.name</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -658,41 +664,35 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Assessment and Plan of Treatment</t>
+          <t>Care Team Members</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core CareTeam Profile</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SDOH Assessment</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>Identifier</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>US Core Practitioner Profile| US Core Patient Profile</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Observation,Condition,QuestionnaireResponse</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Practitioner.identifier</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
           <t>Care Team Members</t>
@@ -703,16 +703,20 @@
           <t>US Core CareTeam Profile</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
+          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>CareTeam.participant</t>
+          <t>PractitionerRole.address, Practitioner.address, RelatedPerson.address</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -732,18 +736,18 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Telecom</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
+          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Practitioner.name, RelatedPerson.name</t>
+          <t>PractitionerRole.telecom, Practitioner.telecom, RelatedPerson.telecom</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -763,49 +767,43 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>Role</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>US Core Practitioner Profile| US Core Patient Profile</t>
+          <t>US Core CareTeam Profile</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Practitioner.identifier</t>
+          <t>CareTeam.participant.role</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Care Team Members</t>
+          <t>Clinical Notes</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
-        </is>
-      </c>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>PractitionerRole.address, Practitioner.address, RelatedPerson.address</t>
+          <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -815,28 +813,28 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Care Team Members</t>
+          <t>Clinical Notes</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Telecom</t>
+          <t>Consultation Note</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>US Core PractitionerRole Profile| US Core Practitioner Profile| US Core Patient Profile| US Core RelatedPerson Profile</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>PractitionerRole.telecom, Practitioner.telecom, RelatedPerson.telecom</t>
+          <t>DocumentReference</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -846,37 +844,35 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Care Team Members</t>
+          <t>Clinical Notes</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Role</t>
+          <t>Discharge Summary Note</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>US Core CareTeam Profile</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>CareTeam.participant.role</t>
+          <t>DocumentReference</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
+      <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
           <t>Clinical Notes</t>
@@ -884,15 +880,23 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+          <t>US Core DocumentReference Profile</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>History &amp; Physical</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>US Core DocumentReference Profile</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
+          <t>DocumentReference</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -907,23 +911,23 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Consultation Note</t>
+          <t>Imaging Narrative</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>DocumentReference</t>
+          <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -938,23 +942,23 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Discharge Summary Note</t>
+          <t>Laboratory Report Narrative</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>DocumentReference</t>
+          <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -969,23 +973,23 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>History &amp; Physical</t>
+          <t>Pathology Report Narrative</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>DocumentReference</t>
+          <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1005,7 +1009,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Imaging Narrative</t>
+          <t>Procedure Note</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1031,54 +1035,60 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Laboratory Report Narrative</t>
+          <t>Progress Note</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+          <t>DocumentReference</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>See Clinical Notes Guidance</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>clinical-notes.html</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="n">
+        <v>4</v>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Clinical Notes</t>
+          <t>Clinical Tests</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Pathology Report Narrative</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
-        </is>
-      </c>
+          <t>Clinical Tests</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
+          <t>Observation, DiagnosticReport</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1088,28 +1098,24 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Clinical Notes</t>
+          <t>Clinical Tests</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Procedure Note</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>US Core DocumentReference Profile|US Core DiagnosticReport Profile for Report and Note exchange</t>
-        </is>
-      </c>
+          <t>Clinical Test</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>DocumentReference,DiagnosticReport</t>
+          <t>Observation, DiagnosticReport</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1119,48 +1125,36 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Clinical Notes</t>
+          <t>Clinical Tests</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Progress Note</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>US Core DocumentReference Profile</t>
-        </is>
-      </c>
+          <t>Clinical Test Result/Report</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>DocumentReference</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>See Clinical Notes Guidance</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>clinical-notes.html</t>
-        </is>
-      </c>
+          <t>Observation, DiagnosticReport</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Clinical Tests</t>
+          <t>Diagnostic Imaging</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1168,11 +1162,7 @@
           <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Clinical Tests</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
@@ -1187,7 +1177,7 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Clinical Tests</t>
+          <t>Diagnostic Imaging</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1197,10 +1187,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Clinical Test</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>Diagnostic Imaging Test</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
@@ -1214,7 +1208,7 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Clinical Tests</t>
+          <t>Diagnostic Imaging</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1224,10 +1218,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Clinical Test Result/Report</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>Diagnostic Imaging Result/Report</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
@@ -1239,24 +1237,28 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1266,28 +1268,28 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging Test</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport</t>
+          <t>Encounter.identifier</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1297,37 +1299,35 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging</t>
+          <t>Encounter</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>US Core Observation Clinical Result Profile| US Core DiagnosticReport Profile for Report and Note Exchange</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Diagnostic Imaging Result/Report</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>US Core Observation Diagnostic Imaging Result Profile| US Core DiagnosticReport Profile for Report and Note exchange</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport</t>
+          <t>Encounter.type</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>6</v>
-      </c>
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
           <t>Encounter</t>
@@ -1335,19 +1335,23 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Diagnosis</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Condition.code</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -1367,7 +1371,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1378,7 +1382,7 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Encounter.identifier</t>
+          <t>Encounter.period</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1398,7 +1402,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1409,7 +1413,7 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Encounter.type</t>
+          <t>Encounter.location.location</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1424,125 +1428,137 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Diagnosis</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core Encounter Profile</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Condition.code</t>
+          <t>Encounter.hospitalization.dischargeDisposition</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="n">
+        <v>7</v>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
+          <t>US Core Location Profile</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Encounter.period</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+          <t>Location.identifier</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>See Facility Information Guidance</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>StructureDefinition-us-core-location.html</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Identifier</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Encounter.location.location</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+          <t>Location.identifier</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>See Facility Information Guidance</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>StructureDefinition-us-core-location.html</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Encounter</t>
+          <t>Facility Information</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>US Core Encounter Profile</t>
+          <t>US Core Location Profile</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Encounter.hospitalization.dischargeDisposition</t>
+          <t>Location.type</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>7</v>
-      </c>
+      <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
           <t>Facility Information</t>
@@ -1553,7 +1569,11 @@
           <t>US Core Location Profile</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
       <c r="E38" t="inlineStr">
         <is>
           <t>US Core Location Profile</t>
@@ -1562,85 +1582,63 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Location.identifier</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>See Facility Information Guidance</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>StructureDefinition-us-core-location.html</t>
-        </is>
-      </c>
+          <t>Location.name</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="n">
+        <v>8</v>
+      </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Facility Information</t>
+          <t>Goals and Preferences</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>US Core Location Profile</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Identifier</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>US Core Location Profile</t>
-        </is>
-      </c>
+          <t>US Core Goal Profile</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Location.identifier</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>See Facility Information Guidance</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>StructureDefinition-us-core-location.html</t>
-        </is>
-      </c>
+          <t>Goal</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Facility Information</t>
+          <t>Goals and Preferences</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>US Core Location Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Patient Goals</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>US Core Location Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Location.type</t>
+          <t>Goal</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -1650,53 +1648,67 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Facility Information</t>
+          <t>Goals and Preferences</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>US Core Location Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>SDOH Goals</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>US Core Location Profile</t>
+          <t>US Core Goal Profile</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Location.name</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+          <t>Goal</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>8</v>
-      </c>
+      <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Goals and Preferences</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
+          <t>US Core Treatment Intervention Preference Profile</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Treatment Intervention Preference</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>US Core Treatment Intervention Preference Profile</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Goal</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -1706,76 +1718,60 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Goals and Preferences</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
+          <t>US Core Care Experience Preference Profile</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Patient Goals</t>
+          <t>Care Experience Preference</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
+          <t>US Core Care Experience Preference Profile</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Goal</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="n">
+        <v>9</v>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Goals</t>
+          <t>Health Insurance Information</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>SDOH Goals</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>US Core Goal Profile</t>
-        </is>
-      </c>
+          <t xml:space="preserve">US Core Coverage Profile | US Core Organization Profile </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Goal</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Coverage | Organization</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>9</v>
-      </c>
+      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
           <t>Health Insurance Information</t>
@@ -1786,12 +1782,20 @@
           <t>US Core Coverage Profile</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Coverage Status</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>US Core Coverage Profile</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Coverage</t>
+          <t>Coverage.status + Coverage.period</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -1811,7 +1815,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Coverage Status</t>
+          <t>Coverage Type</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1822,7 +1826,7 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Coverage.status + Coverage.period</t>
+          <t>Coverage.type</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -1842,7 +1846,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Coverage Type</t>
+          <t>Relationship to Subscriber</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1853,7 +1857,7 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Coverage.type</t>
+          <t>Coverage,relationship</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -1873,7 +1877,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Relationship to Subscriber</t>
+          <t>Member Identifier</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1884,7 +1888,7 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Coverage,relationship</t>
+          <t>Coverage.identifier</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -1904,7 +1908,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Member Identifier</t>
+          <t>Subscriber Identifier</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1915,7 +1919,7 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Coverage.identifier</t>
+          <t>Coverage.subscriberId</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -1935,7 +1939,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Subscriber Identifier</t>
+          <t>Group Number</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1946,7 +1950,7 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Coverage.subscriberId</t>
+          <t>Coverage.class</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -1961,83 +1965,79 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t xml:space="preserve">US Core Coverage Profile | US Core Organization Profile </t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Group Number</t>
+          <t>Payer Identifier</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
+          <t xml:space="preserve">US Core Coverage Profile | US Core Organization Profile </t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Coverage.class</t>
+          <t>Coverage.payer | Organization.identifier</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" t="n">
+        <v>10</v>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Health Insurance Information</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Payer Identifier</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>US Core Coverage Profile</t>
-        </is>
-      </c>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Coverage.payer</t>
+          <t>Observation,Condition,QuestionnaireResponse</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>10</v>
-      </c>
+      <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>Health Concerns</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Observation,Condition,QuestionnaireResponse</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -2047,38 +2047,46 @@
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Health Concerns</t>
+          <t>Functional Status</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2088,7 +2096,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Functional Status</t>
+          <t>Disability Status</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2117,7 +2125,7 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2127,7 +2135,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Disability Status</t>
+          <t>Mental/Cognitive Status</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2141,29 +2149,37 @@
           <t>Observation</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Mental/Cognitive Status</t>
+          <t>Pregnancy Status</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile | US Core Simple Observation Profile</t>
+          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -2179,167 +2195,213 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Pregnancy Status</t>
+          <t>Alcohol Use</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile| US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+          <t>Observation,Condition,QuestionnaireResponse</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Health Status/Assessments</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Smoking Status</t>
+          <t>Substance Use</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>US Core Smoking Status Observation Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+          <t>Observation,Condition,QuestionnaireResponse</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>11</v>
-      </c>
+      <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Immunizations</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Physical Activity</t>
+        </is>
+      </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Immunization</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+          <t>Observation,Condition,QuestionnaireResponse</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Immunizations</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>US Core Immunization Profile</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>SDOH Assessment</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile | US Core Condition Problems and Health Concerns Profile | US Core Observation Screening Assessment Profile | US Core QuestionnaireResponse Profile</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Immunization</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
+          <t>Observation,Condition,QuestionnaireResponse</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>12</v>
-      </c>
+      <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+          <t>US Core Smoking Status Observation Profile</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Smoking Status</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>US Core Smoking Status Observation Profile</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Observation, DiagnosticReport,Specimen</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr"/>
+      <c r="A63" t="n">
+        <v>11</v>
+      </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Immunizations</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Tests</t>
-        </is>
-      </c>
+          <t>US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
+          <t>US Core Immunization Profile</t>
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Observation.code, DiagnosticReport.code</t>
+          <t>Immunization</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -2349,35 +2411,29 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Laboratory</t>
+          <t>Immunizations</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Values/Results</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
-        </is>
-      </c>
+          <t>US Core Immunization Profile</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Observation.value[x], DiagnosticReport.result</t>
+          <t>Immunization</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr"/>
+      <c r="A65" t="n">
+        <v>12</v>
+      </c>
       <c r="B65" t="inlineStr">
         <is>
           <t>Laboratory</t>
@@ -2385,23 +2441,15 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Specimen Type</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
-        </is>
-      </c>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting | US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Observation.specimen, Specimen</t>
+          <t>Observation, DiagnosticReport,Specimen</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -2421,7 +2469,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Result Status</t>
+          <t>Tests</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2432,7 +2480,7 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Observation.status, DiagnosticReport.status</t>
+          <t>Observation.code, DiagnosticReport.code</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -2447,23 +2495,23 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Result Unit of Measure</t>
+          <t>Values/Results</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>(Observation.value.ofType(Quantity)).code</t>
+          <t>Observation.value[x], DiagnosticReport.result</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -2478,23 +2526,23 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Result Reference Range</t>
+          <t>Specimen Type</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core Specimen Profile</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Observation.referenceRange</t>
+          <t>Observation.specimen, Specimen</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -2509,23 +2557,23 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Result Interpretation</t>
+          <t>Result Status</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Laboratory Result Observation Profile| US Core DiagnosticReport Profile for Laboratory Results Reporting</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Observation.interpretation</t>
+          <t>Observation.status, DiagnosticReport.status</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -2540,23 +2588,23 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Specimen Identifier</t>
+          <t>Result Unit of Measure</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Specimen.identifier</t>
+          <t>(Observation.value.ofType(Quantity)).code</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -2571,23 +2619,23 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Specimen Source Site</t>
+          <t>Result Reference Range</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Specimen.collection.bodySite</t>
+          <t>Observation.referenceRange</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -2602,48 +2650,54 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Specimen Condition Acceptability</t>
+          <t>Result Interpretation</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Specimen.condition</t>
+          <t>Observation.interpretation</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>13</v>
-      </c>
+      <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Specimen Identifier</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>MedicationRequest, MedicationDispense, Medication</t>
+          <t>Specimen.identifier</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -2653,98 +2707,84 @@
       <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Specimen Source Site</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Medication.code, MedicationRequest.medication[x]</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>See Medication List Guidance</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>medication-list.html</t>
-        </is>
-      </c>
+          <t>Specimen.collection.bodySite</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Laboratory</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Dose</t>
+          <t>Specimen Condition Acceptability</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+          <t>Specimen.condition</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
+      <c r="A76" t="n">
+        <v>13</v>
+      </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Medical Devices</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Dose Unit of Measure</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
+          <t>US Core Implantable Device Profile</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -2754,35 +2794,37 @@
       <c r="A77" t="inlineStr"/>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Medications</t>
+          <t>Medical Devices</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Indication</t>
+          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Implantable Device Profile</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>MedicationRequest.reasonCode | Medication.reasonReference</t>
+          <t>Device</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr"/>
+      <c r="A78" t="n">
+        <v>14</v>
+      </c>
       <c r="B78" t="inlineStr">
         <is>
           <t>Medications</t>
@@ -2790,23 +2832,15 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Medication Instructions</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
+          <t>US Core MedicationRequest Profile | US Core MedicationDispense Profile | US Core Medication Profile</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>MedicationRequest.dosageInstruction</t>
+          <t>MedicationRequest, MedicationDispense, Medication</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -2821,31 +2855,35 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Medication Profile | US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Medication Adherence</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>US Core Medication Adherence Extension</t>
-        </is>
-      </c>
+          <t>US Core Medication Profile|  US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>MedicationRequest.extension.where(url='Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-medication-adherence')</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
+          <t>Medication.code, MedicationRequest.medication[x]</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>See Medication List Guidance</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>medication-list.html</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
@@ -2856,48 +2894,54 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>US Core MedicationDispense Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Fill Status</t>
+          <t>Dose</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>MedicationDispense</t>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>14</v>
-      </c>
+      <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Dose Unit of Measure</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Patient, Observation</t>
+          <t>MedicationRequest.dosageInstruction.doseAndRate</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -2907,28 +2951,28 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Indication</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>MedicationRequest.reasonCode | Medication.reasonReference</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -2938,28 +2982,28 @@
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Medication Instructions</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Patient.name.family</t>
+          <t>MedicationRequest.dosageInstruction</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -2969,28 +3013,32 @@
       <c r="A84" t="inlineStr"/>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>Medication Adherence</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr"/>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>US Core Medication Adherence Extension</t>
+        </is>
+      </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Patient.name</t>
+          <t>MedicationRequest.extension.where(url='Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-medication-adherence')</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -3000,35 +3048,37 @@
       <c r="A85" t="inlineStr"/>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Patient Demographics</t>
+          <t>Medications</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core MedicationDispense Profile</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Middle Name (including middle initial)</t>
+          <t>Fill Status</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Medication Profile|  US Core MedicationDispense Profile</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Patient.name.given</t>
+          <t>MedicationDispense</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr"/>
+      <c r="A86" t="n">
+        <v>15</v>
+      </c>
       <c r="B86" t="inlineStr">
         <is>
           <t>Patient Demographics</t>
@@ -3036,23 +3086,15 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Suffix</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
+          <t>US Core Patient Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile | US Core Observation Sexual Orientation Profile |US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Patient.name.suffix</t>
+          <t>Patient, Observation</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -3067,12 +3109,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Sex Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3080,14 +3122,10 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>US Core Sex Extension</t>
-        </is>
-      </c>
+      <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-sex')</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
@@ -3107,7 +3145,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Date of Birth</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3118,7 +3156,7 @@
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Patient.birthDate</t>
+          <t>Patient.name.family</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -3138,7 +3176,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Date of Death</t>
+          <t>Previous Name</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3149,7 +3187,7 @@
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>Patient.name</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
@@ -3164,12 +3202,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>US Core Race Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Race</t>
+          <t>Middle Name (including middle initial)</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3177,14 +3215,10 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>US Core Race Extension</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-race')</t>
+          <t>Patient.name.given</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -3199,12 +3233,12 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>Suffix</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3212,14 +3246,10 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>US Core Ethnicity Extension</t>
-        </is>
-      </c>
+      <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity')</t>
+          <t>Patient.name.suffix</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -3234,12 +3264,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+          <t>US Core Patient Profile | US Core Sex Extension</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Tribal Affiliation</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3249,12 +3279,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>US Core Tibal Affiliation Extension</t>
+          <t>US Core Sex Extension</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-tribal-affiliation')</t>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-sex')</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -3269,12 +3299,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Date of Birth</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3282,14 +3312,10 @@
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Gender Identity Extension</t>
-        </is>
-      </c>
+      <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-genderIdentity')</t>
+          <t>Patient.birthDate</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -3304,23 +3330,23 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Date of Death</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.deceased[x]</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -3335,23 +3361,27 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Preferred Language</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>US Core Race Extension</t>
+        </is>
+      </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-race')</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -3366,23 +3396,27 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Ethnicity Extension</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>US Core Ethnicity Extension</t>
+        </is>
+      </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity')</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -3397,23 +3431,27 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Tribal Affiliation Extension</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Tribal Affiliation</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Previous Address</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>US Core Tibal Affiliation Extension</t>
+        </is>
+      </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Patient.address</t>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-tribal-affiliation')</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -3428,23 +3466,27 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
+          <t>US Core Patient Profile | US Core Gender Identity Extension</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Gender Identity</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
           <t>US Core Patient Profile</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>US Core Patient Profile</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Gender Identity Extension</t>
+        </is>
+      </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>Patient.extension.where(url='http://hl7.org/fhir/us/core/StructureDefinition/us-core-genderIdentity')</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -3459,23 +3501,23 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Phone Number</t>
+          <t>Sexual Orientation</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Observation Sexual Orientation Profile</t>
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -3490,23 +3532,23 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Related Person's Name</t>
+          <t>Preferred Language</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr">
         <is>
-          <t>RelatedPerson.name</t>
+          <t>Patient.communication</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -3521,23 +3563,23 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Related Person's Relationship</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>US Core RelatedPerson Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr">
         <is>
-          <t>RelatedPerson.relationship</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -3552,23 +3594,23 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>Previous Address</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.address</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -3583,52 +3625,54 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Occupation Industry</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr"/>
     </row>
     <row r="104">
-      <c r="A104" t="n">
-        <v>15</v>
-      </c>
+      <c r="A104" t="inlineStr"/>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr"/>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Patient Profile</t>
         </is>
       </c>
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Condition</t>
+          <t>Patient.telecom</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -3638,28 +3682,28 @@
       <c r="A105" t="inlineStr"/>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Date of Resolution</t>
+          <t>Related Person's Name</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Condition.abatement[x]</t>
+          <t>RelatedPerson.name</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -3669,32 +3713,28 @@
       <c r="A106" t="inlineStr"/>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core RelatedPerson Profile</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Date of Diagnosis</t>
+          <t>Related Person's Relationship</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>assertedDate Extension</t>
-        </is>
-      </c>
+          <t>US Core RelatedPerson Profile</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Condition.extension.where(url='http://hl7.org/fhir/StructureDefinition/condition-assertedDate') |  Condition.onset[x] | Condition.onsetDate</t>
+          <t>RelatedPerson.relationship</t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
@@ -3704,92 +3744,84 @@
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Problems</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>SDOH Problems/Health Concerns</t>
+          <t>Occupation</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Condition</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="n">
-        <v>16</v>
-      </c>
+      <c r="A108" t="inlineStr"/>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Demographics</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Occupation Industry</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>US Core Observation Occupation Profile</t>
+        </is>
+      </c>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Procedure, ServiceRequest</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr"/>
+      <c r="A109" t="n">
+        <v>16</v>
+      </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Summary and Plan</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Procedure</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>US Core Procedure Profile</t>
-        </is>
-      </c>
+          <t>US Core CarePlan Profile</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Procedure</t>
+          <t>CarePlan</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -3799,59 +3831,57 @@
       <c r="A110" t="inlineStr"/>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Patient Summary and Plan</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
+          <t>US Core CarePlan Profile</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Time of Procedure</t>
+          <t>Assessment and Plan of Treatment</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
+          <t>US Core CarePlan Profile</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Procedure.pertormed[x],DiagnosticReport.effective[x],Immunization.occurrence[x]</t>
+          <t>CarePlan</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr"/>
+      <c r="A111" t="n">
+        <v>17</v>
+      </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Reason for Referral</t>
-        </is>
-      </c>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -3861,164 +3891,158 @@
       <c r="A112" t="inlineStr"/>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Procedures</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>SDOH Interventions</t>
+          <t>Date of Resolution</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr">
         <is>
-          <t>ServiceRequest, Procedure</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>See Screening and Assessments Guidance</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>screening-and-assessments.html</t>
-        </is>
-      </c>
+          <t>Condition.abatement[x]</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
     </row>
     <row r="113">
-      <c r="A113" t="n">
-        <v>17</v>
-      </c>
+      <c r="A113" t="inlineStr"/>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr"/>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Date of Diagnosis</t>
+        </is>
+      </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr"/>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>assertedDate Extension</t>
+        </is>
+      </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Provenance</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>See Basic Provenance Guidance</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>basic-provenance.html</t>
-        </is>
-      </c>
+          <t>Condition.extension.where(url='http://hl7.org/fhir/StructureDefinition/condition-assertedDate') |  Condition.onset[x] | Condition.onsetDate</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Problems</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Author Time Stamp</t>
+          <t>SDOH Problems/Health Concerns</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Provenance.recorded</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr"/>
-      <c r="I114" t="inlineStr"/>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr"/>
+      <c r="A115" t="n">
+        <v>18</v>
+      </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Provenance</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Author Organization</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>US Core Provenance Profile</t>
-        </is>
-      </c>
+          <t>US Core Procedure Profile | US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Provenance.agent</t>
+          <t>Procedure, ServiceRequest</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" t="n">
-        <v>18</v>
-      </c>
+      <c r="A116" t="inlineStr"/>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr"/>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Procedure</t>
+        </is>
+      </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>Procedure</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -4028,53 +4052,59 @@
       <c r="A117" t="inlineStr"/>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s)</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Unique Device Identifier(s) for a Patient's Implantable Device(s)</t>
+          <t>Time of Procedure</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>US Core Implantable Device Profile</t>
+          <t>US Core Procedure Profile|US Core DiagnosticReport Profile for Report and Note Exchange|US Core Immunization Profile</t>
         </is>
       </c>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Device</t>
+          <t>Procedure.pertormed[x],DiagnosticReport.effective[x],Immunization.occurrence[x]</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
     </row>
     <row r="118">
-      <c r="A118" t="n">
-        <v>19</v>
-      </c>
+      <c r="A118" t="inlineStr"/>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>US Core Vital Signs Profile</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr"/>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Reason for Referral</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>ServiceRequest.reasonCode, ServiceRequest.reasonReference</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -4084,90 +4114,104 @@
       <c r="A119" t="inlineStr"/>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Procedures</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
+          <t>US Core ServiceRequest Profile | US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Average Blood Pressure</t>
+          <t>SDOH Interventions</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
+          <t>US Core ServiceRequest Profile|US Core Procedure Profile</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr"/>
+          <t>ServiceRequest, Procedure</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>See Screening and Assessments Guidance</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>screening-and-assessments.html</t>
+        </is>
+      </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr"/>
+      <c r="A120" t="n">
+        <v>19</v>
+      </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Diastolic blood pressure</t>
-        </is>
-      </c>
+          <t>US Core Provenance Profile</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr"/>
+          <t>Provenance</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>See Basic Provenance Guidance</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>basic-provenance.html</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr"/>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Systolic blood pressure</t>
+          <t>Author Time Stamp</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Blood Pressure Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F121" t="inlineStr"/>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Provenance.recorded</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -4177,35 +4221,37 @@
       <c r="A122" t="inlineStr"/>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Provenance</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Body height</t>
+          <t>Author Organization</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Height Profile </t>
+          <t>US Core Provenance Profile</t>
         </is>
       </c>
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Provenance.agent</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr"/>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr"/>
+      <c r="A123" t="n">
+        <v>20</v>
+      </c>
       <c r="B123" t="inlineStr">
         <is>
           <t>Vital Signs</t>
@@ -4213,19 +4259,11 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Body weight</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t xml:space="preserve">US Core Body Weight Profile </t>
-        </is>
-      </c>
+          <t>US Core Vital Signs Profile</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
       <c r="G123" t="inlineStr">
         <is>
@@ -4244,17 +4282,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Heart rate</t>
+          <t>Average Blood Pressure</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Heart Rate Profile </t>
+          <t xml:space="preserve">US Core Average Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F124" t="inlineStr"/>
@@ -4275,17 +4313,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Respiratory rate</t>
+          <t>Diastolic blood pressure</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F125" t="inlineStr"/>
@@ -4306,17 +4344,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Body temperature</t>
+          <t>Systolic blood pressure</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Body Temperature Profile </t>
+          <t xml:space="preserve">US Core Blood Pressure Profile </t>
         </is>
       </c>
       <c r="F126" t="inlineStr"/>
@@ -4337,17 +4375,17 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Pulse oximetry</t>
+          <t>Body height</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Height Profile </t>
         </is>
       </c>
       <c r="F127" t="inlineStr"/>
@@ -4368,17 +4406,17 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Inhaled oxygen concentration</t>
+          <t>Body weight</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+          <t xml:space="preserve">US Core Body Weight Profile </t>
         </is>
       </c>
       <c r="F128" t="inlineStr"/>
@@ -4399,17 +4437,17 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>BMI Percentile (2-20 years old)</t>
+          <t>Heart rate</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+          <t xml:space="preserve">US Core Heart Rate Profile </t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -4430,17 +4468,17 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+          <t>Respiratory rate</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+          <t xml:space="preserve">US Core Respiratory Rate Profile </t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
@@ -4461,17 +4499,17 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+          <t>Body temperature</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+          <t xml:space="preserve">US Core Body Temperature Profile </t>
         </is>
       </c>
       <c r="F131" t="inlineStr"/>
@@ -4482,6 +4520,161 @@
       </c>
       <c r="H131" t="inlineStr"/>
       <c r="I131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Pulse oximetry</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Inhaled oxygen concentration</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pulse Oximetry Profile </t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>BMI Percentile (2-20 years old)</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric BMI for Age Observation Profile </t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr"/>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Weight-for-length Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">US Core Pediatric Weight for Height Observation Profile </t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Occipital Frontal Head Circumference Percentile (Birth - 36 months)</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>US Core Pediatric Head Occipital Frontal Circumference Percentile Profile</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
add USCDI Goals and preferences PART 2 + QA
</commit_message>
<xml_diff>
--- a/input/images/uscdi-table.xlsx
+++ b/input/images/uscdi-table.xlsx
@@ -806,8 +806,16 @@
           <t>DocumentReference,DiagnosticReport</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>See Clinical Notes Guidance</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>clinical-notes.html</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1054,16 +1062,8 @@
           <t>DocumentReference</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>See Clinical Notes Guidance</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>clinical-notes.html</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1465,15 +1465,11 @@
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>US Core Location Profile</t>
-        </is>
-      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Location.identifier</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1515,16 +1511,8 @@
           <t>Location.identifier</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>See Facility Information Guidance</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>StructureDefinition-us-core-location.html</t>
-        </is>
-      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -2843,8 +2831,16 @@
           <t>MedicationRequest, MedicationDispense, Medication</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>See Medication List Guidance</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>medication-list.html</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
@@ -2874,16 +2870,8 @@
           <t>Medication.code, MedicationRequest.medication[x]</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>See Medication List Guidance</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>medication-list.html</t>
-        </is>
-      </c>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>

</xml_diff>